<commit_message>
Change the abreviations of the spectral types in HMXBparamters.xlsx. Added the class to the abreviation
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FC257C-1C98-4D28-BB4B-7ED5EF1AABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A952BC6D-58A3-43E2-91E6-77AA7B9EB6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
@@ -173,19 +173,19 @@
     <t>spectraltype(short)</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>O8</t>
-  </si>
-  <si>
-    <t>O9</t>
-  </si>
-  <si>
-    <t>O6</t>
-  </si>
-  <si>
-    <t>B0</t>
+    <t>B1I</t>
+  </si>
+  <si>
+    <t>O9I</t>
+  </si>
+  <si>
+    <t>B0I</t>
+  </si>
+  <si>
+    <t>O6I</t>
+  </si>
+  <si>
+    <t>O8I</t>
   </si>
 </sst>
 </file>
@@ -308,23 +308,6 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF010101"/>
-        <name val="Calibr  "/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -893,6 +876,23 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF010101"/>
+        <name val="Calibr  "/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1019,31 +1019,31 @@
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{3CDFCB5F-FC45-4284-B98B-6569A50499F1}" name="id" totalsRowLabel="Totaal" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{62D3F204-AEF7-43A9-B874-81735D76945A}" name="spectraltype" dataDxfId="28"/>
-    <tableColumn id="23" xr3:uid="{7502BC3B-5969-4195-B4AC-24D4558256B1}" name="spectraltype(short)" dataDxfId="0"/>
-    <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{219E5554-DD9D-46CB-8AD2-2B86B48E28EB}" name="period" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{24B5BB38-6E79-4DAD-BBD6-13E6D2C56FB3}" name="spinperiod" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{82211366-7646-43A7-9F85-54F391FC2181}" name="eclipseduration" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{B28A1428-2EF7-489F-9BA9-6DF7659F834C}" name="RV" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{393F307D-F090-4F02-A35D-B67885997CB3}" name="Mob" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{3ACE951F-D1A0-490E-8BE0-575186960AAF}" name="Rob" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{9AD61DCF-D27C-478B-BA57-B4FA799B7B26}" name="Mx" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{E59E6B19-CB05-47DF-B143-36DFB8326B7D}" name="parallax" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{102B6FB4-AFA4-426B-AEC7-57E245F806D6}" name="errparallax" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{1BD56C15-699C-46A5-A754-A2FC213343D5}" name="distance" dataDxfId="17">
+    <tableColumn id="23" xr3:uid="{7502BC3B-5969-4195-B4AC-24D4558256B1}" name="spectraltype(short)" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{219E5554-DD9D-46CB-8AD2-2B86B48E28EB}" name="period" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{24B5BB38-6E79-4DAD-BBD6-13E6D2C56FB3}" name="spinperiod" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{82211366-7646-43A7-9F85-54F391FC2181}" name="eclipseduration" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{B28A1428-2EF7-489F-9BA9-6DF7659F834C}" name="RV" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{393F307D-F090-4F02-A35D-B67885997CB3}" name="Mob" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{3ACE951F-D1A0-490E-8BE0-575186960AAF}" name="Rob" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{9AD61DCF-D27C-478B-BA57-B4FA799B7B26}" name="Mx" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{E59E6B19-CB05-47DF-B143-36DFB8326B7D}" name="parallax" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{102B6FB4-AFA4-426B-AEC7-57E245F806D6}" name="errparallax" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{1BD56C15-699C-46A5-A754-A2FC213343D5}" name="distance" dataDxfId="16">
       <calculatedColumnFormula>1/Tabel13[[#This Row],[parallax]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DA27A276-F7A0-4800-B003-962DAE02FA32}" name="distanceBJ" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{5FF56F12-9E90-41C2-85FA-A34AF1447493}" name="luminosity" totalsRowFunction="count" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{8110CBE1-7710-4E52-B49B-B5A0B2559F7E}" name="(B-V)obs" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="15" xr3:uid="{DA27A276-F7A0-4800-B003-962DAE02FA32}" name="distanceBJ" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{5FF56F12-9E90-41C2-85FA-A34AF1447493}" name="luminosity" totalsRowFunction="count" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{8110CBE1-7710-4E52-B49B-B5A0B2559F7E}" name="(B-V)obs" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>Tabel13[[#This Row],[B]]-Tabel13[[#This Row],[V]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C2470258-FA83-48E4-A6E4-09D23A64935C}" name="B" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{747FC6F7-378E-4C67-B0EF-9A8F90B9B1E0}" name="V" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{BA6548C9-6916-4041-92FC-25BA76F00F9A}" name="(B-V)0" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{1E15E01E-5844-436B-B3D8-730C2A5EC9EB}" name="BC" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{2AF1ED53-74F9-4999-8943-ED7C4F197663}" name="mv" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{1D1F0F99-3686-476A-A61F-03B5FA78A47A}" name="Teff" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{C2470258-FA83-48E4-A6E4-09D23A64935C}" name="B" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{747FC6F7-378E-4C67-B0EF-9A8F90B9B1E0}" name="V" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{BA6548C9-6916-4041-92FC-25BA76F00F9A}" name="(B-V)0" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{1E15E01E-5844-436B-B3D8-730C2A5EC9EB}" name="BC" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{2AF1ED53-74F9-4999-8943-ED7C4F197663}" name="mv" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{1D1F0F99-3686-476A-A61F-03B5FA78A47A}" name="Teff" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1349,7 +1349,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1518,7 +1518,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="12">
         <v>1.0028902</v>
@@ -1573,7 +1573,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D4" s="12">
         <v>1.0144804000000001</v>
@@ -1632,7 +1632,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="12">
         <v>0.88019709999999995</v>
@@ -1695,7 +1695,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D6" s="12">
         <v>1.0207037000000001</v>
@@ -1821,7 +1821,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="3">
         <v>0.98579085</v>
@@ -1945,7 +1945,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D10" s="12">
         <v>0.88385309999999995</v>
@@ -2006,7 +2006,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D11" s="12">
         <v>0.99626309999999996</v>
@@ -2065,7 +2065,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="12">
         <v>0.96724250000000001</v>

</xml_diff>

<commit_message>
Made a function to display dataframes stylish
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A952BC6D-58A3-43E2-91E6-77AA7B9EB6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0812A492-4D05-4021-88F4-2261CEC97FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>spectraltype</t>
-  </si>
-  <si>
     <t>ruwe</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>Teff</t>
   </si>
   <si>
-    <t>spectraltype(short)</t>
-  </si>
-  <si>
     <t>B1I</t>
   </si>
   <si>
@@ -186,6 +180,12 @@
   </si>
   <si>
     <t>O8I</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>ST_short</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1018,8 @@
   <autoFilter ref="A1:W12" xr:uid="{92CB420E-405D-4566-9783-CE3C03E82CE3}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{3CDFCB5F-FC45-4284-B98B-6569A50499F1}" name="id" totalsRowLabel="Totaal" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{62D3F204-AEF7-43A9-B874-81735D76945A}" name="spectraltype" dataDxfId="28"/>
-    <tableColumn id="23" xr3:uid="{7502BC3B-5969-4195-B4AC-24D4558256B1}" name="spectraltype(short)" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{62D3F204-AEF7-43A9-B874-81735D76945A}" name="ST" dataDxfId="28"/>
+    <tableColumn id="23" xr3:uid="{7502BC3B-5969-4195-B4AC-24D4558256B1}" name="ST_short" dataDxfId="27"/>
     <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{219E5554-DD9D-46CB-8AD2-2B86B48E28EB}" name="period" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{24B5BB38-6E79-4DAD-BBD6-13E6D2C56FB3}" name="spinperiod" dataDxfId="24"/>
@@ -1349,7 +1349,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1381,70 +1381,70 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -1452,10 +1452,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3">
         <v>0.94464165</v>
@@ -1515,10 +1515,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="12">
         <v>1.0028902</v>
@@ -1570,10 +1570,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="12">
         <v>1.0144804000000001</v>
@@ -1629,10 +1629,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="12">
         <v>0.88019709999999995</v>
@@ -1692,10 +1692,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="12">
         <v>1.0207037000000001</v>
@@ -1755,10 +1755,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="12">
         <v>0.90853119999999998</v>
@@ -1821,7 +1821,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3">
         <v>0.98579085</v>
@@ -1881,10 +1881,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="12">
         <v>0.80819189999999996</v>
@@ -1942,10 +1942,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="12">
         <v>0.88385309999999995</v>
@@ -2003,10 +2003,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="12">
         <v>0.99626309999999996</v>
@@ -2062,10 +2062,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="12">
         <v>0.96724250000000001</v>

</xml_diff>

<commit_message>
Luminosity can now also be calculated for the Bailer-Jones distances and added a comparison of dBJ vs dGAIA
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0812A492-4D05-4021-88F4-2261CEC97FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A02E3-859F-4AAC-9189-5E50BBEF23C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
@@ -308,6 +308,31 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibr  "/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -614,31 +639,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibr  "/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1030,20 +1030,20 @@
     <tableColumn id="9" xr3:uid="{9AD61DCF-D27C-478B-BA57-B4FA799B7B26}" name="Mx" dataDxfId="19"/>
     <tableColumn id="10" xr3:uid="{E59E6B19-CB05-47DF-B143-36DFB8326B7D}" name="parallax" dataDxfId="18"/>
     <tableColumn id="14" xr3:uid="{102B6FB4-AFA4-426B-AEC7-57E245F806D6}" name="errparallax" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{1BD56C15-699C-46A5-A754-A2FC213343D5}" name="distance" dataDxfId="16">
-      <calculatedColumnFormula>1/Tabel13[[#This Row],[parallax]]</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{1BD56C15-699C-46A5-A754-A2FC213343D5}" name="distance" dataDxfId="0">
+      <calculatedColumnFormula>1/Tabel13[[#This Row],[parallax]] * 1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DA27A276-F7A0-4800-B003-962DAE02FA32}" name="distanceBJ" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{5FF56F12-9E90-41C2-85FA-A34AF1447493}" name="luminosity" totalsRowFunction="count" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{8110CBE1-7710-4E52-B49B-B5A0B2559F7E}" name="(B-V)obs" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="15" xr3:uid="{DA27A276-F7A0-4800-B003-962DAE02FA32}" name="distanceBJ" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{5FF56F12-9E90-41C2-85FA-A34AF1447493}" name="luminosity" totalsRowFunction="count" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{8110CBE1-7710-4E52-B49B-B5A0B2559F7E}" name="(B-V)obs" dataDxfId="14" totalsRowDxfId="13">
       <calculatedColumnFormula>Tabel13[[#This Row],[B]]-Tabel13[[#This Row],[V]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C2470258-FA83-48E4-A6E4-09D23A64935C}" name="B" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{747FC6F7-378E-4C67-B0EF-9A8F90B9B1E0}" name="V" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{BA6548C9-6916-4041-92FC-25BA76F00F9A}" name="(B-V)0" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{1E15E01E-5844-436B-B3D8-730C2A5EC9EB}" name="BC" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{2AF1ED53-74F9-4999-8943-ED7C4F197663}" name="mv" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{1D1F0F99-3686-476A-A61F-03B5FA78A47A}" name="Teff" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{C2470258-FA83-48E4-A6E4-09D23A64935C}" name="B" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{747FC6F7-378E-4C67-B0EF-9A8F90B9B1E0}" name="V" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{BA6548C9-6916-4041-92FC-25BA76F00F9A}" name="(B-V)0" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{1E15E01E-5844-436B-B3D8-730C2A5EC9EB}" name="BC" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{2AF1ED53-74F9-4999-8943-ED7C4F197663}" name="mv" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{1D1F0F99-3686-476A-A61F-03B5FA78A47A}" name="Teff" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1348,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DE1212-5B01-4B9B-B604-F1E7439DEFE1}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1482,8 +1482,8 @@
         <v>1.1268352000000001E-2</v>
       </c>
       <c r="N2" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>5.0912049297982236</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>5091.2049297982239</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="6"/>
@@ -1537,8 +1537,8 @@
         <v>2.4794545000000001E-2</v>
       </c>
       <c r="N3" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>250.51413500173422</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>250514.13500173422</v>
       </c>
       <c r="O3" s="9"/>
       <c r="P3" s="15"/>
@@ -1596,8 +1596,8 @@
         <v>2.1808254999999999E-2</v>
       </c>
       <c r="N4" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>225.46909745540654</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>225469.09745540653</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="15"/>
@@ -1659,8 +1659,8 @@
         <v>1.5160984000000001E-2</v>
       </c>
       <c r="N5" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>2.0151539906172817</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>2015.1539906172818</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="15"/>
@@ -1722,8 +1722,8 @@
         <v>1.3698277999999999E-2</v>
       </c>
       <c r="N6" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>7.2088049019485227</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>7208.8049019485225</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="15"/>
@@ -1785,8 +1785,8 @@
         <v>1.5989606999999999E-2</v>
       </c>
       <c r="N7" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>3.9900862091544842</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>3990.0862091544841</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="15"/>
@@ -1848,8 +1848,8 @@
         <v>1.5252326E-2</v>
       </c>
       <c r="N8" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>7.8149758642965557</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>7814.9758642965553</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="15"/>
@@ -1909,8 +1909,8 @@
         <v>2.5948899000000001E-2</v>
       </c>
       <c r="N9" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>1.5804383163952447</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>1580.4383163952448</v>
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="15"/>
@@ -1970,8 +1970,8 @@
         <v>7.313712E-2</v>
       </c>
       <c r="N10" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>4.2987034076373245</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>4298.7034076373247</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="15"/>
@@ -2029,8 +2029,8 @@
         <v>1.7702092999999999E-2</v>
       </c>
       <c r="N11" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>36.402117341361176</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>36402.117341361176</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="17"/>
@@ -2090,8 +2090,8 @@
         <v>1.4949423E-2</v>
       </c>
       <c r="N12" s="9">
-        <f>1/Tabel13[[#This Row],[parallax]]</f>
-        <v>2.2527496407294283</v>
+        <f>1/Tabel13[[#This Row],[parallax]] * 1000</f>
+        <v>2252.7496407294284</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="15"/>

</xml_diff>

<commit_message>
luminosity does not work anymore because the B ST guesses are removed. Added a 2nd file (luminosity2.ipynb) that uses interpolate to guess the values
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A02E3-859F-4AAC-9189-5E50BBEF23C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E243569-F16A-4A81-BA52-D89F18DD4305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>O8.5Iab </t>
   </si>
   <si>
-    <t>O8(f)p</t>
-  </si>
-  <si>
     <t>O9.7Iabpvar </t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>ST_short</t>
+  </si>
+  <si>
+    <t>O8III(f)p</t>
   </si>
 </sst>
 </file>
@@ -308,31 +308,6 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibr  "/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -639,6 +614,31 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibr  "/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1030,20 +1030,20 @@
     <tableColumn id="9" xr3:uid="{9AD61DCF-D27C-478B-BA57-B4FA799B7B26}" name="Mx" dataDxfId="19"/>
     <tableColumn id="10" xr3:uid="{E59E6B19-CB05-47DF-B143-36DFB8326B7D}" name="parallax" dataDxfId="18"/>
     <tableColumn id="14" xr3:uid="{102B6FB4-AFA4-426B-AEC7-57E245F806D6}" name="errparallax" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{1BD56C15-699C-46A5-A754-A2FC213343D5}" name="distance" dataDxfId="0">
+    <tableColumn id="13" xr3:uid="{1BD56C15-699C-46A5-A754-A2FC213343D5}" name="distance" dataDxfId="16">
       <calculatedColumnFormula>1/Tabel13[[#This Row],[parallax]] * 1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DA27A276-F7A0-4800-B003-962DAE02FA32}" name="distanceBJ" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{5FF56F12-9E90-41C2-85FA-A34AF1447493}" name="luminosity" totalsRowFunction="count" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{8110CBE1-7710-4E52-B49B-B5A0B2559F7E}" name="(B-V)obs" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="15" xr3:uid="{DA27A276-F7A0-4800-B003-962DAE02FA32}" name="distanceBJ" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{5FF56F12-9E90-41C2-85FA-A34AF1447493}" name="luminosity" totalsRowFunction="count" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{8110CBE1-7710-4E52-B49B-B5A0B2559F7E}" name="(B-V)obs" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>Tabel13[[#This Row],[B]]-Tabel13[[#This Row],[V]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C2470258-FA83-48E4-A6E4-09D23A64935C}" name="B" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{747FC6F7-378E-4C67-B0EF-9A8F90B9B1E0}" name="V" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{BA6548C9-6916-4041-92FC-25BA76F00F9A}" name="(B-V)0" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{1E15E01E-5844-436B-B3D8-730C2A5EC9EB}" name="BC" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{2AF1ED53-74F9-4999-8943-ED7C4F197663}" name="mv" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{1D1F0F99-3686-476A-A61F-03B5FA78A47A}" name="Teff" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{C2470258-FA83-48E4-A6E4-09D23A64935C}" name="B" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{747FC6F7-378E-4C67-B0EF-9A8F90B9B1E0}" name="V" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{BA6548C9-6916-4041-92FC-25BA76F00F9A}" name="(B-V)0" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{1E15E01E-5844-436B-B3D8-730C2A5EC9EB}" name="BC" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{2AF1ED53-74F9-4999-8943-ED7C4F197663}" name="mv" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{1D1F0F99-3686-476A-A61F-03B5FA78A47A}" name="Teff" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1348,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DE1212-5B01-4B9B-B604-F1E7439DEFE1}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1381,10 +1381,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1444,7 +1444,7 @@
         <v>29</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -1455,7 +1455,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3">
         <v>0.94464165</v>
@@ -1518,7 +1518,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="12">
         <v>1.0028902</v>
@@ -1632,7 +1632,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="12">
         <v>0.88019709999999995</v>
@@ -1758,7 +1758,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="12">
         <v>0.90853119999999998</v>
@@ -1821,7 +1821,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3">
         <v>0.98579085</v>
@@ -1884,7 +1884,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="12">
         <v>0.80819189999999996</v>
@@ -1945,7 +1945,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="12">
         <v>0.88385309999999995</v>
@@ -2003,10 +2003,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D11" s="12">
         <v>0.99626309999999996</v>
@@ -2062,10 +2062,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="12">
         <v>0.96724250000000001</v>

</xml_diff>

<commit_message>
Added 2MASS JHK values to df_hmxb
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C84988E-C1A0-4C18-9F8D-A09A49781ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC534D7-FCEF-4CBF-8C50-E5641B1DB227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t xml:space="preserve">B1Iae </t>
   </si>
   <si>
-    <t xml:space="preserve">O9.7Ia+ </t>
-  </si>
-  <si>
     <t>O8III</t>
   </si>
   <si>
@@ -170,10 +167,13 @@
     <t>B0Iaep</t>
   </si>
   <si>
-    <t>B3sg</t>
-  </si>
-  <si>
     <t>XTE J1855-026</t>
+  </si>
+  <si>
+    <t>B0Ib</t>
+  </si>
+  <si>
+    <t>O5fpe</t>
   </si>
 </sst>
 </file>
@@ -185,8 +185,8 @@
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
     <numFmt numFmtId="166" formatCode="0.00000E+00"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -295,10 +295,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1071,10 +1071,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1095,13 +1095,13 @@
         <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1112,7 +1112,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3">
         <v>0.94464165</v>
@@ -1130,19 +1130,25 @@
       <c r="I2" s="16">
         <v>11.14</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="7">
+        <v>8.5969999999999995</v>
+      </c>
+      <c r="K2" s="7">
+        <v>8.2959999999999994</v>
+      </c>
+      <c r="L2" s="7">
+        <v>8.1069999999999993</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="9">
         <v>1.0028902</v>
@@ -1156,19 +1162,25 @@
       <c r="I3" s="15">
         <v>13.15</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="J3" s="7">
+        <v>13.445</v>
+      </c>
+      <c r="K3" s="7">
+        <v>13.513</v>
+      </c>
+      <c r="L3" s="7">
+        <v>13.474</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="9">
         <v>1.0144804000000001</v>
@@ -1186,19 +1198,25 @@
       <c r="I4" s="7">
         <v>14</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="J4" s="7">
+        <v>14.586</v>
+      </c>
+      <c r="K4" s="7">
+        <v>14.78</v>
+      </c>
+      <c r="L4" s="7">
+        <v>14.75</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="9">
         <v>0.88019709999999995</v>
@@ -1216,19 +1234,25 @@
       <c r="I5" s="7">
         <v>6.87</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="J5" s="7">
+        <v>5.8330000000000002</v>
+      </c>
+      <c r="K5" s="7">
+        <v>5.7050000000000001</v>
+      </c>
+      <c r="L5" s="7">
+        <v>5.5960000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="9">
         <v>1.0207037000000001</v>
@@ -1255,10 +1279,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="9">
         <v>0.90853119999999998</v>
@@ -1276,9 +1300,15 @@
       <c r="I7" s="7">
         <v>10.66</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="J7" s="7">
+        <v>6.7169999999999996</v>
+      </c>
+      <c r="K7" s="7">
+        <v>6.077</v>
+      </c>
+      <c r="L7" s="7">
+        <v>5.6719999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="8" t="s">
@@ -1288,7 +1318,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3">
         <v>0.98579085</v>
@@ -1306,19 +1336,25 @@
       <c r="I8" s="7">
         <v>14.5</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="J8" s="7">
+        <v>10.358000000000001</v>
+      </c>
+      <c r="K8" s="7">
+        <v>9.91</v>
+      </c>
+      <c r="L8" s="7">
+        <v>9.6769999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="9">
         <v>0.80819189999999996</v>
@@ -1334,19 +1370,25 @@
       <c r="I9" s="7">
         <v>6.51</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="J9" s="7">
+        <v>5.7439999999999998</v>
+      </c>
+      <c r="K9" s="7">
+        <v>5.6390000000000002</v>
+      </c>
+      <c r="L9" s="7">
+        <v>5.4960000000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="9">
         <v>0.88385309999999995</v>
@@ -1373,10 +1415,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9">
         <v>0.99626309999999996</v>
@@ -1392,19 +1434,25 @@
       <c r="I11" s="7">
         <v>14.5</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="J11" s="7">
+        <v>13.695</v>
+      </c>
+      <c r="K11" s="7">
+        <v>13.537000000000001</v>
+      </c>
+      <c r="L11" s="7">
+        <v>13.292999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="9">
         <v>0.96724250000000001</v>
@@ -1420,16 +1468,22 @@
       <c r="I12" s="7">
         <v>8.91</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="J12" s="7">
+        <v>6.8719999999999999</v>
+      </c>
+      <c r="K12" s="7">
+        <v>6.6520000000000001</v>
+      </c>
+      <c r="L12" s="7">
+        <v>6.5010000000000003</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="18"/>
@@ -1444,10 +1498,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="18"/>
@@ -1468,10 +1522,10 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="18"/>
@@ -1494,10 +1548,10 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="18"/>

</xml_diff>

<commit_message>
End of the day, update. Nothing changed
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC534D7-FCEF-4CBF-8C50-E5641B1DB227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBEF52C-F29B-41FC-A3BF-53F6F7B4FD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>2S0114+650</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>O5fpe</t>
+  </si>
+  <si>
+    <t>O6.5III</t>
+  </si>
+  <si>
+    <t>B0.5Ib</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1057,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1213,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>29</v>
@@ -1249,7 +1255,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Clean code. And added txt file with a description of how to find distances in the Bailer Jones catalogue.
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F221944F-081E-4651-B62B-EEC92661BD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9200B511-0193-4FBF-AA40-2C8B910B7D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>2S0114+650</t>
   </si>
@@ -59,9 +59,6 @@
     <t>4U1538-52</t>
   </si>
   <si>
-    <t>B0.2Ia</t>
-  </si>
-  <si>
     <t>4U1700-37</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>Barziv et al. (2001)</t>
   </si>
   <si>
-    <t>Kaper (2001) Corbet et al. (2021)</t>
-  </si>
-  <si>
     <t>O6Iaf+</t>
   </si>
   <si>
@@ -177,6 +171,9 @@
   </si>
   <si>
     <t>E(B-V) from van der Meer et al. (2007)</t>
+  </si>
+  <si>
+    <t>B0Ia</t>
   </si>
 </sst>
 </file>
@@ -185,9 +182,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -248,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -263,7 +260,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -275,22 +272,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -335,23 +326,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibr "/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -493,6 +467,23 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibr "/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -619,11 +610,11 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3CDFCB5F-FC45-4284-B98B-6569A50499F1}" name="id" totalsRowLabel="Totaal" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{62D3F204-AEF7-43A9-B874-81735D76945A}" name="ST" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8AA09B7A-CD50-481C-B71F-3707B0FEE3AD}" name="ST_ref" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{24F2687F-2F36-4789-A274-A7BA379BB679}" name="J" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{E63669D6-EF94-4783-8FBA-9518CBF67162}" name="H" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{8C514BBF-8AE2-487A-B056-30A9A8F46585}" name="K" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{8AA09B7A-CD50-481C-B71F-3707B0FEE3AD}" name="ST_ref" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{24F2687F-2F36-4789-A274-A7BA379BB679}" name="J" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{E63669D6-EF94-4783-8FBA-9518CBF67162}" name="H" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{8C514BBF-8AE2-487A-B056-30A9A8F46585}" name="K" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{6AE7B876-5FE3-417F-AC5A-A25DFFEF608C}" name="JHK_ref" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -930,7 +921,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -944,28 +935,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>44</v>
+      <c r="H1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -973,10 +964,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3">
         <v>0.94464165</v>
@@ -990,8 +981,8 @@
       <c r="G2" s="4">
         <v>8.1069999999999993</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>45</v>
+      <c r="H2" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -999,10 +990,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6">
         <v>1.0028902</v>
@@ -1016,8 +1007,8 @@
       <c r="G3" s="4">
         <v>13.474</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>45</v>
+      <c r="H3" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1025,10 +1016,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="6">
         <v>1.0144804000000001</v>
@@ -1042,8 +1033,8 @@
       <c r="G4" s="4">
         <v>14.75</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>45</v>
+      <c r="H4" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1051,10 +1042,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6">
         <v>0.88019709999999995</v>
@@ -1068,8 +1059,8 @@
       <c r="G5" s="4">
         <v>5.5960000000000001</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>45</v>
+      <c r="H5" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1077,10 +1068,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="6">
         <v>1.0207037000000001</v>
@@ -1088,8 +1079,8 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="16" t="s">
-        <v>46</v>
+      <c r="H6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1097,10 +1088,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="6">
         <v>0.90853119999999998</v>
@@ -1114,8 +1105,8 @@
       <c r="G7" s="4">
         <v>5.6719999999999997</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>45</v>
+      <c r="H7" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1123,10 +1114,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3">
         <v>0.98579085</v>
@@ -1140,19 +1131,19 @@
       <c r="G8" s="4">
         <v>9.6769999999999996</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>45</v>
+      <c r="H8" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6">
         <v>0.80819189999999996</v>
@@ -1166,19 +1157,19 @@
       <c r="G9" s="4">
         <v>5.4960000000000004</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>45</v>
+      <c r="H9" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="6">
         <v>0.88385309999999995</v>
@@ -1186,17 +1177,17 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="16"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="6">
         <v>0.99626309999999996</v>
@@ -1210,19 +1201,19 @@
       <c r="G11" s="4">
         <v>13.292999999999999</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>45</v>
+      <c r="H11" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="6">
         <v>0.96724250000000001</v>
@@ -1236,35 +1227,35 @@
       <c r="G12" s="4">
         <v>6.5010000000000003</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>45</v>
+      <c r="H12" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="16"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="12">
@@ -1276,19 +1267,19 @@
       <c r="G14" s="12">
         <v>9.7989999999999995</v>
       </c>
-      <c r="H14" s="16" t="s">
-        <v>45</v>
+      <c r="H14" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="12">
@@ -1300,19 +1291,19 @@
       <c r="G15" s="12">
         <v>10.672000000000001</v>
       </c>
-      <c r="H15" s="16" t="s">
-        <v>45</v>
+      <c r="H15" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="13">
@@ -1324,8 +1315,8 @@
       <c r="G16" s="13">
         <v>10.38</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>45</v>
+      <c r="H16" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did some rearanging of the codes. The mass determination with the HRD is in a separate file and also making the result plots are in their separate file. The code now also correctly calculates the errorbars on Mass radius and Luminosity.
</commit_message>
<xml_diff>
--- a/tables/HMXBparameters.xlsx
+++ b/tables/HMXBparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9200B511-0193-4FBF-AA40-2C8B910B7D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324B2E90-1DD4-4740-8EC6-DB5A52817319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D7EFD20-82E9-4387-B64B-74E2094689FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>2S0114+650</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>B0Ia</t>
+  </si>
+  <si>
+    <t>JHK_err</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -282,11 +285,57 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibr  "/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -605,17 +654,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92CB420E-405D-4566-9783-CE3C03E82CE3}" name="Tabel13" displayName="Tabel13" ref="A1:H16" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
-  <autoFilter ref="A1:H16" xr:uid="{92CB420E-405D-4566-9783-CE3C03E82CE3}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3CDFCB5F-FC45-4284-B98B-6569A50499F1}" name="id" totalsRowLabel="Totaal" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{62D3F204-AEF7-43A9-B874-81735D76945A}" name="ST" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8AA09B7A-CD50-481C-B71F-3707B0FEE3AD}" name="ST_ref" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{24F2687F-2F36-4789-A274-A7BA379BB679}" name="J" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{E63669D6-EF94-4783-8FBA-9518CBF67162}" name="H" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{8C514BBF-8AE2-487A-B056-30A9A8F46585}" name="K" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6AE7B876-5FE3-417F-AC5A-A25DFFEF608C}" name="JHK_ref" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92CB420E-405D-4566-9783-CE3C03E82CE3}" name="Tabel13" displayName="Tabel13" ref="A1:I16" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
+  <autoFilter ref="A1:I16" xr:uid="{92CB420E-405D-4566-9783-CE3C03E82CE3}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3CDFCB5F-FC45-4284-B98B-6569A50499F1}" name="id" totalsRowLabel="Totaal" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{62D3F204-AEF7-43A9-B874-81735D76945A}" name="ST" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{8AA09B7A-CD50-481C-B71F-3707B0FEE3AD}" name="ST_ref" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{6E189503-68AD-41D0-89B7-F8BD4EFBCD13}" name="ruwe" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{24F2687F-2F36-4789-A274-A7BA379BB679}" name="J" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E63669D6-EF94-4783-8FBA-9518CBF67162}" name="H" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{8C514BBF-8AE2-487A-B056-30A9A8F46585}" name="K" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{6AE7B876-5FE3-417F-AC5A-A25DFFEF608C}" name="JHK_ref" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{E8A67492-C113-44E4-9619-55E1A3E9A2BB}" name="JHK_err" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -918,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DE1212-5B01-4B9B-B604-F1E7439DEFE1}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I2" sqref="I2:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,7 +983,7 @@
     <col min="8" max="8" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -958,8 +1008,11 @@
       <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,8 +1037,11 @@
       <c r="H2" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1010,8 +1066,11 @@
       <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1036,8 +1095,11 @@
       <c r="H4" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1062,8 +1124,11 @@
       <c r="H5" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1082,8 +1147,11 @@
       <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1108,8 +1176,11 @@
       <c r="H7" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1134,8 +1205,11 @@
       <c r="H8" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1160,8 +1234,11 @@
       <c r="H9" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1178,8 +1255,11 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1204,8 +1284,11 @@
       <c r="H11" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1230,8 +1313,11 @@
       <c r="H12" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -1246,8 +1332,11 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1270,8 +1359,11 @@
       <c r="H14" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1294,8 +1386,11 @@
       <c r="H15" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1317,6 +1412,9 @@
       </c>
       <c r="H16" s="4" t="s">
         <v>43</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>